<commit_message>
Database connection done to selenium test
</commit_message>
<xml_diff>
--- a/CartData.xlsx
+++ b/CartData.xlsx
@@ -23,7 +23,7 @@
     <t>Total</t>
   </si>
   <si>
-    <t>290.47</t>
+    <t>1079.13</t>
   </si>
 </sst>
 </file>
@@ -68,7 +68,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -87,22 +87,38 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="n">
-        <v>289.0</v>
+        <v>389.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="B3" t="n">
-        <v>1.47</v>
+        <v>3.99</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="s">
+      <c r="A4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B4" t="n">
+        <v>312.5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B5" t="n">
+        <v>365.66</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>